<commit_message>
Digit coding from Hyunji.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/digits_HS.xlsx
+++ b/raw-data-prep/raw_data/digits_HS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>L_ring_length</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Subject</t>
+  </si>
+  <si>
+    <t>left: index longer, right: ring longer</t>
+  </si>
+  <si>
+    <t>left: ring longer, right: index longer</t>
   </si>
 </sst>
 </file>
@@ -387,11 +393,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,6 +442,862 @@
       </c>
       <c r="J1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>919.9</v>
+      </c>
+      <c r="C2">
+        <v>84.07</v>
+      </c>
+      <c r="D2">
+        <v>916.3</v>
+      </c>
+      <c r="E2">
+        <v>88.5</v>
+      </c>
+      <c r="F2">
+        <v>889</v>
+      </c>
+      <c r="G2">
+        <v>78.45</v>
+      </c>
+      <c r="H2">
+        <v>895.7</v>
+      </c>
+      <c r="I2">
+        <v>80.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>131</v>
+      </c>
+      <c r="B3">
+        <v>898.9</v>
+      </c>
+      <c r="C3">
+        <v>87.39</v>
+      </c>
+      <c r="D3">
+        <v>902.4</v>
+      </c>
+      <c r="E3">
+        <v>84.34</v>
+      </c>
+      <c r="F3">
+        <v>891.8</v>
+      </c>
+      <c r="G3">
+        <v>86.4</v>
+      </c>
+      <c r="H3">
+        <v>897</v>
+      </c>
+      <c r="I3">
+        <v>89.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <v>850.6</v>
+      </c>
+      <c r="C4">
+        <v>58.55</v>
+      </c>
+      <c r="D4">
+        <v>850.3</v>
+      </c>
+      <c r="E4">
+        <v>88.52</v>
+      </c>
+      <c r="F4">
+        <v>860.2</v>
+      </c>
+      <c r="G4">
+        <v>88.8</v>
+      </c>
+      <c r="H4">
+        <v>872.4</v>
+      </c>
+      <c r="I4">
+        <v>85.73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>151</v>
+      </c>
+      <c r="B5">
+        <v>898.6</v>
+      </c>
+      <c r="C5">
+        <v>85.66</v>
+      </c>
+      <c r="D5">
+        <v>870.7</v>
+      </c>
+      <c r="E5">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="F5">
+        <v>856.2</v>
+      </c>
+      <c r="G5">
+        <v>82.08</v>
+      </c>
+      <c r="H5">
+        <v>883.8</v>
+      </c>
+      <c r="I5">
+        <v>86.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>231</v>
+      </c>
+      <c r="B6">
+        <v>925.5</v>
+      </c>
+      <c r="C6">
+        <v>85.04</v>
+      </c>
+      <c r="D6">
+        <v>867.3</v>
+      </c>
+      <c r="E6">
+        <v>88.48</v>
+      </c>
+      <c r="F6">
+        <v>841.6</v>
+      </c>
+      <c r="G6">
+        <v>86.46</v>
+      </c>
+      <c r="H6">
+        <v>916.2</v>
+      </c>
+      <c r="I6">
+        <v>85.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>148</v>
+      </c>
+      <c r="B7">
+        <v>873.1</v>
+      </c>
+      <c r="C7">
+        <v>89.28</v>
+      </c>
+      <c r="D7">
+        <v>859.8</v>
+      </c>
+      <c r="E7">
+        <v>76.209999999999994</v>
+      </c>
+      <c r="F7">
+        <v>882.4</v>
+      </c>
+      <c r="G7">
+        <v>79.62</v>
+      </c>
+      <c r="H7">
+        <v>880.1</v>
+      </c>
+      <c r="I7">
+        <v>89.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>375</v>
+      </c>
+      <c r="B8">
+        <v>936.2</v>
+      </c>
+      <c r="C8">
+        <v>79.66</v>
+      </c>
+      <c r="D8">
+        <v>923.3</v>
+      </c>
+      <c r="E8">
+        <v>85.96</v>
+      </c>
+      <c r="F8">
+        <v>916</v>
+      </c>
+      <c r="G8">
+        <v>83.42</v>
+      </c>
+      <c r="H8">
+        <v>924.8</v>
+      </c>
+      <c r="I8">
+        <v>83.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>425</v>
+      </c>
+      <c r="B9">
+        <v>902.1</v>
+      </c>
+      <c r="C9">
+        <v>84.53</v>
+      </c>
+      <c r="D9">
+        <v>882.1</v>
+      </c>
+      <c r="E9">
+        <v>88.69</v>
+      </c>
+      <c r="F9">
+        <v>862.4</v>
+      </c>
+      <c r="G9">
+        <v>85.74</v>
+      </c>
+      <c r="H9">
+        <v>934.4</v>
+      </c>
+      <c r="I9">
+        <v>82.81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>426</v>
+      </c>
+      <c r="B10">
+        <v>950.6</v>
+      </c>
+      <c r="C10">
+        <v>83.23</v>
+      </c>
+      <c r="D10">
+        <v>963.8</v>
+      </c>
+      <c r="E10">
+        <v>82.73</v>
+      </c>
+      <c r="F10">
+        <v>946.5</v>
+      </c>
+      <c r="G10">
+        <v>88.18</v>
+      </c>
+      <c r="H10">
+        <v>965</v>
+      </c>
+      <c r="I10">
+        <v>83.1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>427</v>
+      </c>
+      <c r="B11">
+        <v>869</v>
+      </c>
+      <c r="C11">
+        <v>85.25</v>
+      </c>
+      <c r="D11">
+        <v>880.5</v>
+      </c>
+      <c r="E11">
+        <v>88.05</v>
+      </c>
+      <c r="F11">
+        <v>838.4</v>
+      </c>
+      <c r="G11">
+        <v>88.22</v>
+      </c>
+      <c r="H11">
+        <v>892</v>
+      </c>
+      <c r="I11">
+        <v>80.58</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>428</v>
+      </c>
+      <c r="B12">
+        <v>999.2</v>
+      </c>
+      <c r="C12">
+        <v>88.97</v>
+      </c>
+      <c r="D12">
+        <v>919.2</v>
+      </c>
+      <c r="E12">
+        <v>87.13</v>
+      </c>
+      <c r="F12">
+        <v>939.3</v>
+      </c>
+      <c r="G12">
+        <v>87.01</v>
+      </c>
+      <c r="H12">
+        <v>966.6</v>
+      </c>
+      <c r="I12">
+        <v>88.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>429</v>
+      </c>
+      <c r="B13">
+        <v>849.4</v>
+      </c>
+      <c r="C13">
+        <v>84.87</v>
+      </c>
+      <c r="D13">
+        <v>788.4</v>
+      </c>
+      <c r="E13">
+        <v>88.11</v>
+      </c>
+      <c r="F13">
+        <v>790.9</v>
+      </c>
+      <c r="G13">
+        <v>83.61</v>
+      </c>
+      <c r="H13">
+        <v>846.2</v>
+      </c>
+      <c r="I13">
+        <v>88.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>430</v>
+      </c>
+      <c r="B14">
+        <v>935.4</v>
+      </c>
+      <c r="C14">
+        <v>83.86</v>
+      </c>
+      <c r="D14">
+        <v>850.2</v>
+      </c>
+      <c r="E14">
+        <v>88.92</v>
+      </c>
+      <c r="F14">
+        <v>850.1</v>
+      </c>
+      <c r="G14">
+        <v>89.19</v>
+      </c>
+      <c r="H14">
+        <v>941.3</v>
+      </c>
+      <c r="I14">
+        <v>81.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>431</v>
+      </c>
+      <c r="B15">
+        <v>974</v>
+      </c>
+      <c r="C15">
+        <v>79.56</v>
+      </c>
+      <c r="D15">
+        <v>948.8</v>
+      </c>
+      <c r="E15">
+        <v>87.7</v>
+      </c>
+      <c r="F15">
+        <v>938.3</v>
+      </c>
+      <c r="G15">
+        <v>88.66</v>
+      </c>
+      <c r="H15">
+        <v>976.2</v>
+      </c>
+      <c r="I15">
+        <v>84.71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>432</v>
+      </c>
+      <c r="B16">
+        <v>995.3</v>
+      </c>
+      <c r="C16">
+        <v>87.12</v>
+      </c>
+      <c r="D16">
+        <v>996</v>
+      </c>
+      <c r="E16">
+        <v>89.77</v>
+      </c>
+      <c r="F16">
+        <v>1034.5999999999999</v>
+      </c>
+      <c r="G16">
+        <v>88.12</v>
+      </c>
+      <c r="H16">
+        <v>1003.6</v>
+      </c>
+      <c r="I16">
+        <v>81.290000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>433</v>
+      </c>
+      <c r="B17">
+        <v>919.5</v>
+      </c>
+      <c r="C17">
+        <v>81.75</v>
+      </c>
+      <c r="D17">
+        <v>873.2</v>
+      </c>
+      <c r="E17">
+        <v>88.82</v>
+      </c>
+      <c r="F17">
+        <v>859.5</v>
+      </c>
+      <c r="G17">
+        <v>82.45</v>
+      </c>
+      <c r="H17">
+        <v>898.6</v>
+      </c>
+      <c r="I17">
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>434</v>
+      </c>
+      <c r="B18">
+        <v>1031.0999999999999</v>
+      </c>
+      <c r="C18">
+        <v>85.55</v>
+      </c>
+      <c r="D18">
+        <v>946.2</v>
+      </c>
+      <c r="E18">
+        <v>86.12</v>
+      </c>
+      <c r="F18">
+        <v>966.3</v>
+      </c>
+      <c r="G18">
+        <v>86.08</v>
+      </c>
+      <c r="H18">
+        <v>1034.4000000000001</v>
+      </c>
+      <c r="I18">
+        <v>86.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>435</v>
+      </c>
+      <c r="B19">
+        <v>905.9</v>
+      </c>
+      <c r="C19">
+        <v>86.33</v>
+      </c>
+      <c r="D19">
+        <v>906.5</v>
+      </c>
+      <c r="E19">
+        <v>82.65</v>
+      </c>
+      <c r="F19">
+        <v>881.3</v>
+      </c>
+      <c r="G19">
+        <v>85.9</v>
+      </c>
+      <c r="H19">
+        <v>908.7</v>
+      </c>
+      <c r="I19">
+        <v>83.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>436</v>
+      </c>
+      <c r="B20">
+        <v>869.4</v>
+      </c>
+      <c r="C20">
+        <v>79.930000000000007</v>
+      </c>
+      <c r="D20">
+        <v>820.1</v>
+      </c>
+      <c r="E20">
+        <v>89.3</v>
+      </c>
+      <c r="F20">
+        <v>818.4</v>
+      </c>
+      <c r="G20">
+        <v>85.59</v>
+      </c>
+      <c r="H20">
+        <v>880.5</v>
+      </c>
+      <c r="I20">
+        <v>81.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>437</v>
+      </c>
+      <c r="B21">
+        <v>982.5</v>
+      </c>
+      <c r="C21">
+        <v>88.13</v>
+      </c>
+      <c r="D21">
+        <v>988.5</v>
+      </c>
+      <c r="E21">
+        <v>79.510000000000005</v>
+      </c>
+      <c r="F21">
+        <v>988.1</v>
+      </c>
+      <c r="G21">
+        <v>86.29</v>
+      </c>
+      <c r="H21">
+        <v>1003</v>
+      </c>
+      <c r="I21">
+        <v>81.510000000000005</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>438</v>
+      </c>
+      <c r="B22">
+        <v>959</v>
+      </c>
+      <c r="C22">
+        <v>84.13</v>
+      </c>
+      <c r="D22">
+        <v>894.2</v>
+      </c>
+      <c r="E22">
+        <v>88.72</v>
+      </c>
+      <c r="F22">
+        <v>868.1</v>
+      </c>
+      <c r="G22">
+        <v>89.34</v>
+      </c>
+      <c r="H22">
+        <v>948.4</v>
+      </c>
+      <c r="I22">
+        <v>83.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>439</v>
+      </c>
+      <c r="B23">
+        <v>938.9</v>
+      </c>
+      <c r="C23">
+        <v>84.13</v>
+      </c>
+      <c r="D23">
+        <v>917.1</v>
+      </c>
+      <c r="E23">
+        <v>87.25</v>
+      </c>
+      <c r="F23">
+        <v>929.2</v>
+      </c>
+      <c r="G23">
+        <v>87.04</v>
+      </c>
+      <c r="H23">
+        <v>924.7</v>
+      </c>
+      <c r="I23">
+        <v>85.66</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>440</v>
+      </c>
+      <c r="B24">
+        <v>921.1</v>
+      </c>
+      <c r="C24">
+        <v>82.89</v>
+      </c>
+      <c r="D24">
+        <v>857.6</v>
+      </c>
+      <c r="E24">
+        <v>86.52</v>
+      </c>
+      <c r="F24">
+        <v>870.9</v>
+      </c>
+      <c r="G24">
+        <v>87.37</v>
+      </c>
+      <c r="H24">
+        <v>938.5</v>
+      </c>
+      <c r="I24">
+        <v>83.27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>441</v>
+      </c>
+      <c r="B25">
+        <v>886.6</v>
+      </c>
+      <c r="C25">
+        <v>84.17</v>
+      </c>
+      <c r="D25">
+        <v>858.1</v>
+      </c>
+      <c r="E25">
+        <v>89.07</v>
+      </c>
+      <c r="F25">
+        <v>864.1</v>
+      </c>
+      <c r="G25">
+        <v>89.07</v>
+      </c>
+      <c r="H25">
+        <v>889.3</v>
+      </c>
+      <c r="I25">
+        <v>82.64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>442</v>
+      </c>
+      <c r="B26">
+        <v>964.5</v>
+      </c>
+      <c r="C26">
+        <v>81.53</v>
+      </c>
+      <c r="D26">
+        <v>904.2</v>
+      </c>
+      <c r="E26">
+        <v>88.86</v>
+      </c>
+      <c r="F26">
+        <v>886.2</v>
+      </c>
+      <c r="G26">
+        <v>84.43</v>
+      </c>
+      <c r="H26">
+        <v>966</v>
+      </c>
+      <c r="I26">
+        <v>86.32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>443</v>
+      </c>
+      <c r="B27">
+        <v>870.1</v>
+      </c>
+      <c r="C27">
+        <v>77.66</v>
+      </c>
+      <c r="D27">
+        <v>850.4</v>
+      </c>
+      <c r="E27">
+        <v>86.7</v>
+      </c>
+      <c r="F27">
+        <v>840.7</v>
+      </c>
+      <c r="G27">
+        <v>86.32</v>
+      </c>
+      <c r="H27">
+        <v>861.7</v>
+      </c>
+      <c r="I27">
+        <v>77.739999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>444</v>
+      </c>
+      <c r="B28">
+        <v>886.8</v>
+      </c>
+      <c r="C28">
+        <v>84.05</v>
+      </c>
+      <c r="D28">
+        <v>924.1</v>
+      </c>
+      <c r="E28">
+        <v>87.15</v>
+      </c>
+      <c r="F28">
+        <v>866.9</v>
+      </c>
+      <c r="G28">
+        <v>86.23</v>
+      </c>
+      <c r="H28">
+        <v>895.9</v>
+      </c>
+      <c r="I28">
+        <v>78.209999999999994</v>
+      </c>
+      <c r="J28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>445</v>
+      </c>
+      <c r="B29">
+        <v>840.7</v>
+      </c>
+      <c r="C29">
+        <v>80.83</v>
+      </c>
+      <c r="D29">
+        <v>808</v>
+      </c>
+      <c r="E29">
+        <v>89.72</v>
+      </c>
+      <c r="F29">
+        <v>804.7</v>
+      </c>
+      <c r="G29">
+        <v>87.58</v>
+      </c>
+      <c r="H29">
+        <v>812.8</v>
+      </c>
+      <c r="I29">
+        <v>80.650000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>446</v>
+      </c>
+      <c r="B30">
+        <v>960</v>
+      </c>
+      <c r="C30">
+        <v>84.74</v>
+      </c>
+      <c r="D30">
+        <v>934.2</v>
+      </c>
+      <c r="E30">
+        <v>88.77</v>
+      </c>
+      <c r="F30">
+        <v>922.3</v>
+      </c>
+      <c r="G30">
+        <v>88.63</v>
+      </c>
+      <c r="H30">
+        <v>974.5</v>
+      </c>
+      <c r="I30">
+        <v>83.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>